<commit_message>
update uitgevoerd op dimensietabellem
</commit_message>
<xml_diff>
--- a/Week 4/Dimensietabellen.xlsx
+++ b/Week 4/Dimensietabellen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\School\Jaar 2\Semester 4\dedsportfolio\Week 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F209E9C-FFBC-41F1-97CF-E910D0BF16E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5755EEFA-E2F4-4799-A346-226ABA33B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81FA8BFE-3ABB-440C-9C8D-D1A7BF216359}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{81FA8BFE-3ABB-440C-9C8D-D1A7BF216359}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>PRODUCT</t>
   </si>
@@ -120,28 +120,6 @@
   </si>
   <si>
     <t>PRODUCT_TYPE_EN</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>sales_staff_code</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Aptos"/>
-        <family val="2"/>
-      </rPr>
-      <t>, first_name, last_name, extension, work_phone, fax, email, date_hired</t>
-    </r>
   </si>
   <si>
     <r>
@@ -169,12 +147,6 @@
     <t>zone</t>
   </si>
   <si>
-    <t>ADDRESS</t>
-  </si>
-  <si>
-    <t>address1, address2</t>
-  </si>
-  <si>
     <t>code, name</t>
   </si>
   <si>
@@ -187,24 +159,12 @@
     <t>meer op meer</t>
   </si>
   <si>
-    <t xml:space="preserve">retailer_code, </t>
-  </si>
-  <si>
-    <t>COMPANY_NAME</t>
-  </si>
-  <si>
-    <t>RETAILER_TYPE</t>
-  </si>
-  <si>
-    <t>retailer_type_code, retailer_type_en</t>
+    <t>RETAILER_CODE</t>
   </si>
   <si>
     <t>Meetwaarden:</t>
   </si>
   <si>
-    <t xml:space="preserve">PRODUCT_PRICE = PRODUCTION_COST * MARGIN + PRODUCTION_COST = PRICE </t>
-  </si>
-  <si>
     <t>YEAR = DATE.to_year()</t>
   </si>
   <si>
@@ -215,6 +175,80 @@
   </si>
   <si>
     <t>QUARTER = DATE.to_quarter()</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>sales_staff_code</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t>, first_name, last_name, extension, work_phone, fax, email, date_hired, address1, address2</t>
+    </r>
+  </si>
+  <si>
+    <t>RETAILTER_TYPE</t>
+  </si>
+  <si>
+    <t>retailer_type_en, retailer_type_code</t>
+  </si>
+  <si>
+    <t>SEGMENT</t>
+  </si>
+  <si>
+    <t>segment_code, segment_name</t>
+  </si>
+  <si>
+    <t>GENDER</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>country_code, country_en</t>
+  </si>
+  <si>
+    <r>
+      <t>retailer_site_code,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> retailer_contact_code, first_name, last_name, extension, fax, email,phone, active_indicator, language, retailer_name, segment_description, job_position, address1, address2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PRODUCT_PRICE = PRODUCTION_COST * MARGIN + PRODUCTION_COST </t>
+  </si>
+  <si>
+    <t>code_mr, company_name</t>
   </si>
 </sst>
 </file>
@@ -258,7 +292,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -531,11 +565,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -642,38 +750,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -749,20 +848,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,7 +913,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>369903</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>147961</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1211,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3416C82A-03A7-4D65-BCC2-EB736D497023}">
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,7 +1385,7 @@
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1297,7 +1417,7 @@
     </row>
     <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
@@ -1306,12 +1426,12 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1332,105 +1452,165 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4162C3-BB57-43DA-B219-7A381FAB0F94}">
-  <dimension ref="B1:F10"/>
+  <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="5" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="29" t="s">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="72" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="74"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="F3" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="35"/>
+      <c r="H3" s="47"/>
+    </row>
+    <row r="4" spans="2:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="40"/>
+      <c r="F4" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="40"/>
+      <c r="H4" s="47"/>
+    </row>
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="33"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
-    </row>
-    <row r="5" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="35"/>
-    </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="38" t="s">
+      <c r="C5" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="46"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="39"/>
-      <c r="F6" s="40"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="43"/>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="38"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="46"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="32"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="37"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="80"/>
+      <c r="C7" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="35"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="80"/>
+      <c r="C8" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
+      <c r="G8" s="40"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="80"/>
+      <c r="C9" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="37"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="81"/>
+      <c r="C10" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="77" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="79"/>
+    </row>
+    <row r="12" spans="2:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="62"/>
+      <c r="G12" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="B3:C8"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D6:F6"/>
+  <mergeCells count="14">
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="C10:G10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B12:G12"/>
+    <mergeCell ref="B2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1439,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B7BD93-E4BB-4508-AF58-A791762C28CD}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView zoomScale="103" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,12 +1635,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="77" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
+      <c r="B1" s="71" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
@@ -1471,29 +1651,29 @@
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="60"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="76"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="63"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="16"/>
       <c r="C5" s="26" t="s">
         <v>13</v>
@@ -1502,7 +1682,7 @@
       <c r="E5" s="28"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="76"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="16"/>
       <c r="C6" s="23" t="s">
         <v>2</v>
@@ -1511,25 +1691,25 @@
       <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="16"/>
-      <c r="C7" s="70" t="s">
+      <c r="C7" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="72"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="76"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="16"/>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="69"/>
-      <c r="E8" s="68"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="65"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="16"/>
       <c r="C9" s="14" t="s">
         <v>16</v>
@@ -1538,7 +1718,7 @@
       <c r="E9" s="15"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="76"/>
+      <c r="A10" s="70"/>
       <c r="B10" s="16"/>
       <c r="C10" s="19" t="s">
         <v>2</v>
@@ -1547,7 +1727,7 @@
       <c r="E10" s="20"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="76"/>
+      <c r="A11" s="70"/>
       <c r="B11" s="16"/>
       <c r="C11" s="26" t="s">
         <v>14</v>
@@ -1556,57 +1736,37 @@
       <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="76"/>
+      <c r="A12" s="70"/>
       <c r="B12" s="16"/>
       <c r="C12" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="24"/>
       <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="76"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="76"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="73" t="s">
+      <c r="A13" s="70"/>
+      <c r="B13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="14" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="75"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
-      <c r="B15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-    </row>
-    <row r="16" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="A3:A15"/>
+  <mergeCells count="16">
+    <mergeCell ref="A3:A13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
@@ -1617,11 +1777,11 @@
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:E12"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="B4:B12"/>
     <mergeCell ref="C5:E5"/>
     <mergeCell ref="C6:E6"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1649,13 +1809,13 @@
       <c r="F2" s="31"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="46"/>
     </row>
     <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="38" t="s">
@@ -1665,7 +1825,7 @@
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
       <c r="F4" s="40"/>
-      <c r="G4" s="50"/>
+      <c r="G4" s="47"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
@@ -1675,7 +1835,7 @@
       <c r="D5" s="34"/>
       <c r="E5" s="34"/>
       <c r="F5" s="35"/>
-      <c r="G5" s="57"/>
+      <c r="G5" s="54"/>
     </row>
     <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="38" t="s">
@@ -1685,25 +1845,25 @@
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
       <c r="F6" s="40"/>
-      <c r="G6" s="57"/>
+      <c r="G6" s="54"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="53"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
     </row>
     <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
@@ -1715,37 +1875,37 @@
       <c r="F9" s="32"/>
     </row>
     <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="64" t="s">
+      <c r="B10" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="63"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sterdiagram af hoop ik
</commit_message>
<xml_diff>
--- a/Week 4/Dimensietabellen.xlsx
+++ b/Week 4/Dimensietabellen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Will\Desktop\School\Jaar 2\Semester 4\dedsportfolio\Week 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William\Desktop\School\jaar 2\semester 4\dedsportfolio\Week 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCC82A1-5103-4778-B083-926451E3D868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7E78BC-DB3A-4F15-B928-CDD165CCC829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{81FA8BFE-3ABB-440C-9C8D-D1A7BF216359}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{81FA8BFE-3ABB-440C-9C8D-D1A7BF216359}"/>
   </bookViews>
   <sheets>
     <sheet name="FEITENMODEL" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
   <si>
     <t>PRODUCT</t>
   </si>
@@ -386,12 +386,69 @@
   <si>
     <t>code, upper_age, lower_age</t>
   </si>
+  <si>
+    <t>SALES_TARGETData</t>
+  </si>
+  <si>
+    <t>SALES_TARGETData_id</t>
+  </si>
+  <si>
+    <t>SALES_TARGETData_year</t>
+  </si>
+  <si>
+    <t>SALES_TARGETData_period</t>
+  </si>
+  <si>
+    <t>SALES_TARGETData_cost</t>
+  </si>
+  <si>
+    <t>SALES_TARGETData_margin</t>
+  </si>
+  <si>
+    <t>SALES_TARGETData_profit</t>
+  </si>
+  <si>
+    <t>TRAINING_year</t>
+  </si>
+  <si>
+    <t>ORDER_profit_margin</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST</t>
+  </si>
+  <si>
+    <t>SALES_INVENTORY_LEVELS</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST_product_number</t>
+  </si>
+  <si>
+    <t>SALES_INVENTORY_LEVELS_product_number</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST_year</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST_month</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST_expected_volume</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST_inventory_count</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST_inventory_year</t>
+  </si>
+  <si>
+    <t>SALES_PRODUCT_FORECAST_inventory_month</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,6 +481,15 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -837,7 +903,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -907,12 +973,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -939,24 +999,192 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -965,237 +1193,120 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1228,6 +1339,129 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1252,13 +1486,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1305,13 +1539,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1356,16 +1590,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2171700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>285750</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1380,8 +1614,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4305300" y="3943350"/>
-          <a:ext cx="1743075" cy="666750"/>
+          <a:off x="8572500" y="8940800"/>
+          <a:ext cx="4076700" cy="5327650"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1409,15 +1643,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1254125</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1433,8 +1667,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="8172450" y="3962400"/>
-          <a:ext cx="1162050" cy="1238250"/>
+          <a:off x="12985750" y="10937875"/>
+          <a:ext cx="1358900" cy="3022600"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1464,13 +1698,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1517,13 +1751,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1538,9 +1772,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7239000" y="5553075"/>
-          <a:ext cx="0" cy="2276475"/>
+        <a:xfrm flipH="1">
+          <a:off x="11741150" y="10922000"/>
+          <a:ext cx="6350" cy="4492625"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1568,15 +1802,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2247900</xdr:colOff>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3105150</xdr:colOff>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1592,8 +1826,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3209925" y="8191500"/>
-          <a:ext cx="9525" cy="1181100"/>
+          <a:off x="4181475" y="17554575"/>
+          <a:ext cx="857250" cy="1323975"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1622,15 +1856,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1447800</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:colOff>1428750</xdr:colOff>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1666875</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1645,8 +1879,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="3200400" y="10448925"/>
-          <a:ext cx="219075" cy="914400"/>
+          <a:off x="3362325" y="15678150"/>
+          <a:ext cx="238125" cy="1143000"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1674,15 +1908,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2628900</xdr:colOff>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1698,8 +1932,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6800850" y="8029575"/>
-          <a:ext cx="771525" cy="2571750"/>
+          <a:off x="9029700" y="17545050"/>
+          <a:ext cx="1209675" cy="2714625"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1729,13 +1963,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>89</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1753,6 +1987,271 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="7677150" y="11858625"/>
           <a:ext cx="200025" cy="895350"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1447800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2257425</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Rechte verbindingslijn met pijl 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9090A655-2E4B-41D4-B211-FD1FF01D51B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3381375" y="3352800"/>
+          <a:ext cx="809625" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Rechte verbindingslijn met pijl 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{713665B0-1BED-42DC-B24A-08A3453D4113}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="14744700" y="15306675"/>
+          <a:ext cx="1428750" cy="733425"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1409700</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3095625</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>333375</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Rechte verbindingslijn met pijl 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A151DC72-0F81-41AD-B80B-64A4C2452117}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3330575" y="14052550"/>
+          <a:ext cx="1685925" cy="2314575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1514475</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Rechte verbindingslijn met pijl 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E9D0741-6186-4FDF-AAB5-02EA52A3E3B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3448050" y="2771775"/>
+          <a:ext cx="9525" cy="447675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1314450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Rechte verbindingslijn met pijl 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{710D01A4-85AB-4243-9A15-25DDC3EE5CEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7705725" y="2771775"/>
+          <a:ext cx="9525" cy="447675"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2209,729 +2708,879 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F38E616-B02C-492F-99D0-A4EE7AAA0E86}">
-  <dimension ref="C5:U61"/>
+  <dimension ref="C1:U93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="78" workbookViewId="0">
-      <selection activeCell="V26" sqref="V26"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="46.85546875" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21.42578125" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" customWidth="1"/>
     <col min="21" max="21" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:21" ht="15.75" thickBot="1"/>
-    <row r="6" spans="3:21" ht="15.75" thickBot="1">
-      <c r="C6" s="70" t="s">
+    <row r="1" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="151" t="s">
+        <v>104</v>
+      </c>
+      <c r="F3" s="151" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="37"/>
+      <c r="F4" s="37"/>
+    </row>
+    <row r="5" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="37" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="72"/>
-      <c r="O6" s="112" t="s">
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="G9" s="64"/>
+      <c r="O9" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="P6" s="113"/>
-      <c r="Q6" s="113"/>
-      <c r="R6" s="113"/>
-      <c r="S6" s="113"/>
-      <c r="T6" s="113"/>
-      <c r="U6" s="114"/>
-    </row>
-    <row r="7" spans="3:21" ht="27.75" customHeight="1">
-      <c r="C7" s="10" t="s">
+      <c r="P9" s="71"/>
+      <c r="Q9" s="71"/>
+      <c r="R9" s="71"/>
+      <c r="S9" s="71"/>
+      <c r="T9" s="71"/>
+      <c r="U9" s="72"/>
+    </row>
+    <row r="10" spans="3:21" ht="27" x14ac:dyDescent="0.25">
+      <c r="C10" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="21" t="s">
+      <c r="F10" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G10" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" s="38" t="s">
+      <c r="Q10" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="39"/>
-      <c r="S7" s="38" t="s">
+      <c r="R10" s="46"/>
+      <c r="S10" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="T7" s="39"/>
-      <c r="U7" s="8" t="s">
+      <c r="T10" s="46"/>
+      <c r="U10" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="3:21" ht="54.75" thickBot="1">
-      <c r="C8" s="76" t="s">
+    <row r="11" spans="3:21" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="169" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="D11" s="169" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E11" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="76" t="s">
+      <c r="F11" s="169" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O11" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="P11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q8" s="40" t="s">
+      <c r="Q11" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="R8" s="41"/>
-      <c r="S8" s="40" t="s">
+      <c r="R11" s="11"/>
+      <c r="S11" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="T8" s="41"/>
-      <c r="U8" s="11" t="s">
+      <c r="T11" s="11"/>
+      <c r="U11" s="11" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="3:21" ht="40.5">
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="21" t="s">
+    <row r="12" spans="3:21" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="169"/>
+      <c r="D12" s="169"/>
+      <c r="E12" s="169"/>
+      <c r="F12" s="169"/>
+      <c r="G12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="O9" s="8" t="s">
+      <c r="O12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="63" t="s">
+      <c r="P12" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="63"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="63"/>
-      <c r="U9" s="64"/>
-    </row>
-    <row r="10" spans="3:21" ht="15.75" thickBot="1">
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="22" t="s">
+      <c r="Q12" s="60"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="164"/>
+    </row>
+    <row r="13" spans="3:21" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="186"/>
+      <c r="D13" s="186"/>
+      <c r="E13" s="186"/>
+      <c r="F13" s="186"/>
+      <c r="G13" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="O10" s="107" t="s">
+      <c r="O13" s="178" t="s">
         <v>49</v>
       </c>
-      <c r="P10" s="43" t="s">
+      <c r="P13" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="Q10" s="43"/>
-      <c r="R10" s="43"/>
-      <c r="S10" s="43"/>
-      <c r="T10" s="43"/>
-      <c r="U10" s="44"/>
-    </row>
-    <row r="11" spans="3:21" ht="15.75" thickBot="1">
-      <c r="C11" s="73" t="s">
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="30"/>
+      <c r="U13" s="32"/>
+    </row>
+    <row r="14" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="167" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
-      <c r="K11" s="110" t="s">
+      <c r="D14" s="168"/>
+      <c r="E14" s="168"/>
+      <c r="F14" s="168"/>
+      <c r="G14" s="158"/>
+      <c r="K14" s="135" t="s">
         <v>75</v>
       </c>
-      <c r="L11" s="111"/>
-      <c r="O11" s="107"/>
-      <c r="P11" s="38" t="s">
+      <c r="L14" s="136"/>
+      <c r="O14" s="178"/>
+      <c r="P14" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="66"/>
-    </row>
-    <row r="12" spans="3:21" ht="15.75" thickBot="1">
-      <c r="C12" s="115" t="s">
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="46"/>
+      <c r="T14" s="46"/>
+      <c r="U14" s="47"/>
+    </row>
+    <row r="15" spans="3:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="117"/>
-      <c r="K12" s="36" t="s">
+      <c r="D15" s="80"/>
+      <c r="E15" s="183"/>
+      <c r="F15" s="183"/>
+      <c r="G15" s="184"/>
+      <c r="K15" s="194" t="s">
         <v>76</v>
       </c>
-      <c r="L12" s="37"/>
-      <c r="O12" s="107"/>
-      <c r="P12" s="40" t="s">
+      <c r="L15" s="185"/>
+      <c r="O15" s="178"/>
+      <c r="P15" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
-      <c r="U12" s="41"/>
-    </row>
-    <row r="13" spans="3:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="K13" s="118" t="s">
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="11"/>
+    </row>
+    <row r="16" spans="3:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K16" s="180" t="s">
         <v>77</v>
       </c>
-      <c r="L13" s="119"/>
-      <c r="O13" s="107"/>
-      <c r="P13" s="38" t="s">
+      <c r="L16" s="181"/>
+      <c r="O16" s="178"/>
+      <c r="P16" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="66"/>
-    </row>
-    <row r="14" spans="3:21" ht="14.25" customHeight="1" thickBot="1">
-      <c r="K14" s="25"/>
-      <c r="L14" s="26"/>
-      <c r="O14" s="107"/>
-      <c r="P14" s="42" t="s">
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="47"/>
+    </row>
+    <row r="17" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K17" s="187"/>
+      <c r="L17" s="188"/>
+      <c r="O17" s="178"/>
+      <c r="P17" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="Q14" s="43"/>
-      <c r="R14" s="43"/>
-      <c r="S14" s="43"/>
-      <c r="T14" s="43"/>
-      <c r="U14" s="44"/>
-    </row>
-    <row r="15" spans="3:21" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="K15" s="36" t="s">
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="32"/>
+    </row>
+    <row r="18" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="159" t="s">
         <v>78</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="O15" s="107"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="34"/>
-    </row>
-    <row r="16" spans="3:21" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="K16" s="23" t="s">
+      <c r="L18" s="160"/>
+      <c r="O18" s="178"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="30"/>
+      <c r="T18" s="30"/>
+      <c r="U18" s="32"/>
+    </row>
+    <row r="19" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K19" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="L16" s="24"/>
-      <c r="O16" s="107"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="34"/>
-    </row>
-    <row r="17" spans="4:21" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="K17" s="23" t="s">
+      <c r="L19" s="24"/>
+      <c r="O19" s="178"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="32"/>
+    </row>
+    <row r="20" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K20" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="L17" s="24"/>
-      <c r="O17" s="107"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="34"/>
-    </row>
-    <row r="18" spans="4:21" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="K18" s="23" t="s">
+      <c r="L20" s="24"/>
+      <c r="O20" s="178"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="32"/>
+    </row>
+    <row r="21" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="L18" s="24"/>
-      <c r="O18" s="107"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="34"/>
-    </row>
-    <row r="19" spans="4:21" ht="15.75" hidden="1" customHeight="1" thickBot="1">
-      <c r="K19" s="23"/>
-      <c r="L19" s="24"/>
-      <c r="O19" s="107"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="32"/>
-      <c r="R19" s="32"/>
-      <c r="S19" s="32"/>
-      <c r="T19" s="32"/>
-      <c r="U19" s="34"/>
-    </row>
-    <row r="20" spans="4:21" ht="15.75" hidden="1" thickBot="1">
-      <c r="K20" s="49" t="s">
+      <c r="L21" s="24"/>
+      <c r="O21" s="178"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="32"/>
+    </row>
+    <row r="22" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K22" s="23"/>
+      <c r="L22" s="24"/>
+      <c r="O22" s="178"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="30"/>
+      <c r="T22" s="30"/>
+      <c r="U22" s="32"/>
+    </row>
+    <row r="23" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" s="24"/>
+      <c r="O23" s="179"/>
+      <c r="P23" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q23" s="39"/>
+      <c r="R23" s="39"/>
+      <c r="S23" s="39"/>
+      <c r="T23" s="39"/>
+      <c r="U23" s="11"/>
+    </row>
+    <row r="24" spans="4:21" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K24" s="23"/>
+      <c r="L24" s="24"/>
+      <c r="O24" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="60"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="60"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="61"/>
+    </row>
+    <row r="25" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K25" s="161" t="s">
+        <v>72</v>
+      </c>
+      <c r="L25" s="161"/>
+      <c r="O25" s="189" t="s">
+        <v>47</v>
+      </c>
+      <c r="P25" s="190"/>
+      <c r="Q25" s="190"/>
+      <c r="R25" s="190"/>
+      <c r="S25" s="190"/>
+      <c r="T25" s="190"/>
+      <c r="U25" s="154"/>
+    </row>
+    <row r="26" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="182" t="s">
+        <v>73</v>
+      </c>
+      <c r="L26" s="182"/>
+      <c r="O26" s="44"/>
+      <c r="P26" s="44"/>
+      <c r="Q26" s="44"/>
+      <c r="R26" s="44"/>
+      <c r="S26" s="44"/>
+      <c r="T26" s="44"/>
+      <c r="U26" s="44"/>
+    </row>
+    <row r="27" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K27" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="L27" s="24"/>
+      <c r="O27" s="153"/>
+      <c r="P27" s="153"/>
+      <c r="Q27" s="153"/>
+      <c r="R27" s="153"/>
+      <c r="S27" s="153"/>
+      <c r="T27" s="153"/>
+      <c r="U27" s="153"/>
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="O28" s="153"/>
+      <c r="P28" s="153"/>
+      <c r="Q28" s="153"/>
+      <c r="R28" s="153"/>
+      <c r="S28" s="153"/>
+      <c r="T28" s="153"/>
+      <c r="U28" s="153"/>
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="O29" s="153"/>
+      <c r="P29" s="153"/>
+      <c r="Q29" s="153"/>
+      <c r="R29" s="153"/>
+      <c r="S29" s="153"/>
+      <c r="T29" s="153"/>
+      <c r="U29" s="153"/>
+    </row>
+    <row r="30" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="36" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="150"/>
+    </row>
+    <row r="32" spans="4:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="151" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="37"/>
+      <c r="K33" s="156"/>
+      <c r="L33" s="156"/>
+    </row>
+    <row r="34" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="T34" s="28"/>
+    </row>
+    <row r="35" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="O35" s="152"/>
+      <c r="P35" s="152"/>
+      <c r="Q35" s="152"/>
+      <c r="R35" s="152"/>
+      <c r="S35" s="152"/>
+      <c r="T35" s="28"/>
+    </row>
+    <row r="36" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="37"/>
+      <c r="O36" s="152"/>
+      <c r="P36" s="152"/>
+      <c r="Q36" s="152"/>
+      <c r="R36" s="152"/>
+      <c r="S36" s="152"/>
+      <c r="T36" s="28"/>
+    </row>
+    <row r="37" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="O37" s="152"/>
+      <c r="P37" s="152"/>
+      <c r="Q37" s="152"/>
+      <c r="R37" s="152"/>
+      <c r="S37" s="152"/>
+      <c r="T37" s="28"/>
+    </row>
+    <row r="38" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="O38" s="152"/>
+      <c r="P38" s="152"/>
+      <c r="Q38" s="152"/>
+      <c r="R38" s="152"/>
+      <c r="S38" s="152"/>
+      <c r="T38" s="28"/>
+    </row>
+    <row r="39" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="37" t="s">
+        <v>99</v>
+      </c>
+      <c r="O39" s="152"/>
+      <c r="P39" s="152"/>
+      <c r="Q39" s="152"/>
+      <c r="R39" s="152"/>
+      <c r="S39" s="152"/>
+      <c r="T39" s="28"/>
+    </row>
+    <row r="40" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="37"/>
+      <c r="O40" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="P40" s="71"/>
+      <c r="Q40" s="71"/>
+      <c r="R40" s="71"/>
+      <c r="S40" s="72"/>
+      <c r="T40" s="28"/>
+    </row>
+    <row r="41" spans="4:20" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="O41" s="163" t="s">
+        <v>19</v>
+      </c>
+      <c r="P41" s="60"/>
+      <c r="Q41" s="60"/>
+      <c r="R41" s="60"/>
+      <c r="S41" s="164"/>
+      <c r="T41" s="29"/>
+    </row>
+    <row r="42" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="L20" s="49"/>
-      <c r="O20" s="108"/>
-      <c r="P20" s="65" t="s">
+      <c r="O42" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="P42" s="39"/>
+      <c r="Q42" s="39"/>
+      <c r="R42" s="39"/>
+      <c r="S42" s="11"/>
+      <c r="T42" s="19"/>
+    </row>
+    <row r="43" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="O43" s="45" t="s">
+        <v>21</v>
+      </c>
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="47"/>
+      <c r="T43" s="19"/>
+    </row>
+    <row r="44" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="156"/>
+      <c r="E44" s="156"/>
+      <c r="O44" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="P44" s="39"/>
+      <c r="Q44" s="39"/>
+      <c r="R44" s="39"/>
+      <c r="S44" s="11"/>
+      <c r="T44" s="19"/>
+    </row>
+    <row r="45" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D45" s="156"/>
+      <c r="E45" s="156"/>
+      <c r="O45" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="P45" s="46"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="46"/>
+      <c r="S45" s="47"/>
+      <c r="T45" s="30"/>
+    </row>
+    <row r="46" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="156"/>
+      <c r="E46" s="156"/>
+      <c r="O46" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="P46" s="39"/>
+      <c r="Q46" s="39"/>
+      <c r="R46" s="39"/>
+      <c r="S46" s="11"/>
+      <c r="T46" s="30"/>
+    </row>
+    <row r="47" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D47" s="156"/>
+      <c r="E47" s="156"/>
+      <c r="O47" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="P47" s="20"/>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="20"/>
+      <c r="S47" s="2"/>
+      <c r="T47" s="20"/>
+    </row>
+    <row r="48" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="156"/>
+      <c r="E48" s="156"/>
+      <c r="O48" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="P48" s="42"/>
+      <c r="Q48" s="42"/>
+      <c r="R48" s="42"/>
+      <c r="S48" s="43"/>
+      <c r="T48" s="31"/>
+    </row>
+    <row r="49" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D49" s="156"/>
+      <c r="E49" s="156"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+    </row>
+    <row r="50" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K50" s="135" t="s">
+        <v>82</v>
+      </c>
+      <c r="L50" s="136"/>
+    </row>
+    <row r="51" spans="4:15" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G51" s="156"/>
+      <c r="H51" s="156"/>
+      <c r="K51" s="162" t="s">
+        <v>83</v>
+      </c>
+      <c r="L51" s="162"/>
+    </row>
+    <row r="52" spans="4:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G52" s="156"/>
+      <c r="H52" s="156"/>
+      <c r="K52" s="159"/>
+      <c r="L52" s="160"/>
+    </row>
+    <row r="53" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="165" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="166"/>
+      <c r="F53" s="166"/>
+      <c r="G53" s="157"/>
+      <c r="H53" s="156"/>
+      <c r="K53" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="L53" s="27"/>
+    </row>
+    <row r="54" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="167" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="168"/>
+      <c r="G54" s="158"/>
+      <c r="H54" s="156"/>
+      <c r="K54" s="159"/>
+      <c r="L54" s="160"/>
+    </row>
+    <row r="55" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="169" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="170" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="171"/>
+      <c r="G55" s="155"/>
+      <c r="H55" s="156"/>
+      <c r="K55" s="81" t="s">
+        <v>74</v>
+      </c>
+      <c r="L55" s="82"/>
+    </row>
+    <row r="56" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D56" s="169"/>
+      <c r="E56" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="49"/>
+      <c r="G56" s="50"/>
+      <c r="H56" s="156"/>
+      <c r="K56" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="L56" s="26"/>
+    </row>
+    <row r="57" spans="4:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="169"/>
+      <c r="E57" s="172" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" s="173"/>
+      <c r="G57" s="174"/>
+      <c r="K57" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="L57" s="26"/>
+    </row>
+    <row r="58" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D58" s="169"/>
+      <c r="E58" s="175" t="s">
+        <v>15</v>
+      </c>
+      <c r="F58" s="176"/>
+      <c r="G58" s="177"/>
+    </row>
+    <row r="59" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="169"/>
+      <c r="E59" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" s="52"/>
+      <c r="G59" s="53"/>
+    </row>
+    <row r="60" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="169"/>
+      <c r="E60" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="49"/>
+      <c r="G60" s="50"/>
+      <c r="O60" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D61" s="169"/>
+      <c r="E61" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" s="52"/>
+      <c r="G61" s="53"/>
+      <c r="O61" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="4:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="169"/>
+      <c r="E62" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="F62" s="49"/>
+      <c r="G62" s="50"/>
+      <c r="O62" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="4:15" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D63" s="169"/>
+      <c r="E63" s="172" t="s">
         <v>28</v>
       </c>
-      <c r="Q20" s="65"/>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
-      <c r="U20" s="41"/>
-    </row>
-    <row r="21" spans="4:21" ht="15.75" thickBot="1">
-      <c r="K21" s="49" t="s">
-        <v>72</v>
-      </c>
-      <c r="L21" s="49"/>
-      <c r="O21" s="104" t="s">
-        <v>30</v>
-      </c>
-      <c r="P21" s="105"/>
-      <c r="Q21" s="105"/>
-      <c r="R21" s="105"/>
-      <c r="S21" s="105"/>
-      <c r="T21" s="105"/>
-      <c r="U21" s="106"/>
-    </row>
-    <row r="22" spans="4:21" ht="39" customHeight="1" thickBot="1">
-      <c r="K22" s="120" t="s">
+      <c r="F63" s="173"/>
+      <c r="G63" s="174"/>
+    </row>
+    <row r="64" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D64" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E64" s="55"/>
+      <c r="F64" s="55"/>
+      <c r="G64" s="56"/>
+    </row>
+    <row r="65" spans="4:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D65" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="E65" s="58"/>
+      <c r="F65" s="58"/>
+      <c r="G65" s="3"/>
+    </row>
+    <row r="72" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E73" s="191"/>
+    </row>
+    <row r="74" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D74" s="148" t="s">
+        <v>87</v>
+      </c>
+      <c r="E74" s="192"/>
+    </row>
+    <row r="75" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D75" s="34"/>
+      <c r="E75" s="191"/>
+    </row>
+    <row r="76" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D76" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E76" s="193"/>
+    </row>
+    <row r="77" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D77" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="L22" s="120"/>
-      <c r="O22" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="P22" s="57"/>
-      <c r="Q22" s="57"/>
-      <c r="R22" s="57"/>
-      <c r="S22" s="57"/>
-      <c r="T22" s="57"/>
-      <c r="U22" s="58"/>
-    </row>
-    <row r="23" spans="4:21" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D23" s="70" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="71"/>
-      <c r="F23" s="71"/>
-      <c r="G23" s="72"/>
-      <c r="K23" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="L23" s="49"/>
-    </row>
-    <row r="24" spans="4:21" ht="15.75" thickBot="1">
-      <c r="D24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="73" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="74"/>
-      <c r="G24" s="75"/>
-      <c r="K24" s="109"/>
-      <c r="L24" s="109"/>
-    </row>
-    <row r="25" spans="4:21" ht="15.75" thickBot="1">
-      <c r="D25" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" s="77" t="s">
-        <v>2</v>
-      </c>
-      <c r="F25" s="78"/>
-      <c r="G25" s="79"/>
-      <c r="O25" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="60"/>
-      <c r="S25" s="61"/>
-      <c r="T25" s="30"/>
-    </row>
-    <row r="26" spans="4:21">
-      <c r="D26" s="76"/>
-      <c r="E26" s="80" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="81"/>
-      <c r="G26" s="82"/>
-      <c r="O26" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" s="63"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="63"/>
-      <c r="S26" s="64"/>
-      <c r="T26" s="31"/>
-    </row>
-    <row r="27" spans="4:21" ht="15.75" thickBot="1">
-      <c r="D27" s="76"/>
-      <c r="E27" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="F27" s="84"/>
-      <c r="G27" s="85"/>
-      <c r="O27" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="41"/>
-      <c r="T27" s="19"/>
-    </row>
-    <row r="28" spans="4:21">
-      <c r="D28" s="76"/>
-      <c r="E28" s="86" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="87"/>
-      <c r="G28" s="88"/>
-      <c r="O28" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="39"/>
-      <c r="R28" s="39"/>
-      <c r="S28" s="66"/>
-      <c r="T28" s="19"/>
-    </row>
-    <row r="29" spans="4:21" ht="15.75" thickBot="1">
-      <c r="D29" s="76"/>
-      <c r="E29" s="89" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" s="90"/>
-      <c r="G29" s="91"/>
-      <c r="O29" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="P29" s="65"/>
-      <c r="Q29" s="65"/>
-      <c r="R29" s="65"/>
-      <c r="S29" s="41"/>
-      <c r="T29" s="19"/>
-    </row>
-    <row r="30" spans="4:21">
-      <c r="D30" s="76"/>
-      <c r="E30" s="92" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="93"/>
-      <c r="G30" s="94"/>
-      <c r="O30" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="P30" s="68"/>
-      <c r="Q30" s="68"/>
-      <c r="R30" s="68"/>
-      <c r="S30" s="69"/>
-      <c r="T30" s="32"/>
-    </row>
-    <row r="31" spans="4:21" ht="15.75" thickBot="1">
-      <c r="D31" s="76"/>
-      <c r="E31" s="95" t="s">
-        <v>2</v>
-      </c>
-      <c r="F31" s="96"/>
-      <c r="G31" s="97"/>
-      <c r="O31" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="51"/>
-      <c r="S31" s="52"/>
-      <c r="T31" s="32"/>
-    </row>
-    <row r="32" spans="4:21">
-      <c r="D32" s="76"/>
-      <c r="E32" s="80" t="s">
-        <v>14</v>
-      </c>
-      <c r="F32" s="81"/>
-      <c r="G32" s="82"/>
-      <c r="O32" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="P32" s="54"/>
-      <c r="Q32" s="54"/>
-      <c r="R32" s="54"/>
-      <c r="S32" s="55"/>
-      <c r="T32" s="20"/>
-    </row>
-    <row r="33" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D33" s="76"/>
-      <c r="E33" s="83" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33" s="84"/>
-      <c r="G33" s="85"/>
-      <c r="O33" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="P33" s="57"/>
-      <c r="Q33" s="57"/>
-      <c r="R33" s="57"/>
-      <c r="S33" s="58"/>
-      <c r="T33" s="33"/>
-    </row>
-    <row r="34" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D34" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="E34" s="99"/>
-      <c r="F34" s="99"/>
-      <c r="G34" s="100"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-    </row>
-    <row r="35" spans="4:20" ht="26.25" customHeight="1" thickBot="1">
-      <c r="D35" s="101" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="102"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="103"/>
-      <c r="K35" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="L35" s="47"/>
-    </row>
-    <row r="36" spans="4:20" ht="15.75" thickBot="1">
-      <c r="K36" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="L36" s="48"/>
-    </row>
-    <row r="37" spans="4:20" ht="15.75" thickBot="1">
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
-    </row>
-    <row r="38" spans="4:20" ht="15.75" thickBot="1">
-      <c r="K38" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="L38" s="29"/>
-    </row>
-    <row r="39" spans="4:20" ht="15.75" thickBot="1">
-      <c r="K39" s="45"/>
-      <c r="L39" s="46"/>
-    </row>
-    <row r="40" spans="4:20" ht="15.75" thickBot="1">
-      <c r="K40" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="L40" s="49"/>
-    </row>
-    <row r="41" spans="4:20" ht="15.75" thickBot="1">
-      <c r="K41" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="L41" s="28"/>
-    </row>
-    <row r="42" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D42" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="46"/>
-      <c r="K42" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="L42" s="28"/>
-    </row>
-    <row r="43" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D43" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="37"/>
-    </row>
-    <row r="44" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D44" s="45"/>
-      <c r="E44" s="46"/>
-    </row>
-    <row r="45" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D45" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="E45" s="37"/>
-    </row>
-    <row r="46" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D46" s="36" t="s">
+      <c r="E77" s="193"/>
+    </row>
+    <row r="78" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D78" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E78" s="193"/>
+    </row>
+    <row r="79" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G80" s="135" t="s">
+        <v>89</v>
+      </c>
+      <c r="H80" s="136"/>
+    </row>
+    <row r="81" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G81" s="148" t="s">
+        <v>90</v>
+      </c>
+      <c r="H81" s="149"/>
+    </row>
+    <row r="82" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G82" s="34"/>
+      <c r="H82" s="35"/>
+    </row>
+    <row r="83" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G83" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="H83" s="24"/>
+    </row>
+    <row r="84" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G84" s="23"/>
+      <c r="H84" s="24"/>
+    </row>
+    <row r="85" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D85" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G85" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E46" s="37"/>
-    </row>
-    <row r="47" spans="4:20" ht="15.75" thickBot="1">
-      <c r="D47" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="E47" s="37"/>
-    </row>
-    <row r="48" spans="4:20" ht="15.75" thickBot="1"/>
-    <row r="49" spans="4:8" ht="15.75" thickBot="1">
-      <c r="G49" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="H49" s="46"/>
-    </row>
-    <row r="50" spans="4:8" ht="15.75" thickBot="1">
-      <c r="G50" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="H50" s="37"/>
-    </row>
-    <row r="51" spans="4:8" ht="15.75" thickBot="1">
-      <c r="G51" s="45"/>
-      <c r="H51" s="46"/>
-    </row>
-    <row r="52" spans="4:8" ht="15.75" thickBot="1">
-      <c r="G52" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="H52" s="37"/>
-    </row>
-    <row r="53" spans="4:8" ht="15.75" thickBot="1">
-      <c r="D53" s="12" t="s">
+      <c r="H85" s="24"/>
+    </row>
+    <row r="86" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D86" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G53" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H53" s="37"/>
-    </row>
-    <row r="54" spans="4:8" ht="15.75" thickBot="1">
-      <c r="D54" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G54" s="36" t="s">
+      <c r="G86" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="H54" s="37"/>
-    </row>
-    <row r="55" spans="4:8" ht="30.75" thickBot="1">
-      <c r="D55" s="18" t="s">
+      <c r="H86" s="24"/>
+    </row>
+    <row r="87" spans="4:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="58" spans="4:8" ht="15.75" thickBot="1"/>
-    <row r="59" spans="4:8" ht="15.75" thickBot="1">
-      <c r="H59" s="12" t="s">
+    <row r="90" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H91" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="60" spans="4:8">
-      <c r="H60" s="13" t="s">
+    <row r="92" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H92" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="4:8" ht="30.75" thickBot="1">
-      <c r="H61" s="18" t="s">
+    <row r="93" spans="4:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H93" s="18" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="P9:U9"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="D34:G34"/>
-    <mergeCell ref="D35:G35"/>
-    <mergeCell ref="O21:U21"/>
-    <mergeCell ref="O22:U22"/>
-    <mergeCell ref="O10:O20"/>
-    <mergeCell ref="P10:U10"/>
-    <mergeCell ref="P11:U11"/>
-    <mergeCell ref="P12:U12"/>
-    <mergeCell ref="P13:U13"/>
-    <mergeCell ref="P20:U20"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="D23:G23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="D25:D33"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="O31:S31"/>
-    <mergeCell ref="O32:S32"/>
-    <mergeCell ref="O33:S33"/>
-    <mergeCell ref="O25:S25"/>
-    <mergeCell ref="O26:S26"/>
-    <mergeCell ref="O27:S27"/>
-    <mergeCell ref="O28:S28"/>
-    <mergeCell ref="O29:S29"/>
-    <mergeCell ref="O30:S30"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K40:L40"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K39:L39"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="P14:U14"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="K15:L15"/>
+  <mergeCells count="9">
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="O25:T25"/>
+    <mergeCell ref="G80:H80"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="O40:S40"/>
+    <mergeCell ref="O9:U9"/>
+    <mergeCell ref="C9:G9"/>
+    <mergeCell ref="K14:L14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2946,7 +3595,7 @@
       <selection activeCell="B2" sqref="B2:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
@@ -2955,135 +3604,135 @@
     <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B1" s="132" t="s">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="147" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="132"/>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B2" s="70" t="s">
+      <c r="C1" s="147"/>
+      <c r="D1" s="147"/>
+      <c r="E1" s="147"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="131"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="64"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="146"/>
       <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75"/>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A4" s="131"/>
-      <c r="B4" s="76" t="s">
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="146"/>
+      <c r="B4" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="78"/>
-      <c r="E4" s="79"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="131"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="80" t="s">
+      <c r="D4" s="102"/>
+      <c r="E4" s="103"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="146"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="104" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="81"/>
-      <c r="E5" s="82"/>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A6" s="131"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="83" t="s">
+      <c r="D5" s="105"/>
+      <c r="E5" s="106"/>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="146"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="84"/>
-      <c r="E6" s="85"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="131"/>
-      <c r="B7" s="76"/>
-      <c r="C7" s="86" t="s">
+      <c r="D6" s="108"/>
+      <c r="E6" s="109"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="146"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="110" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="87"/>
-      <c r="E7" s="88"/>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A8" s="131"/>
-      <c r="B8" s="76"/>
-      <c r="C8" s="89" t="s">
+      <c r="D7" s="111"/>
+      <c r="E7" s="112"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="146"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="90"/>
-      <c r="E8" s="91"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="131"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="92" t="s">
+      <c r="D8" s="114"/>
+      <c r="E8" s="115"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="146"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="116" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="94"/>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A10" s="131"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="95" t="s">
+      <c r="D9" s="117"/>
+      <c r="E9" s="118"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="146"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="96"/>
-      <c r="E10" s="97"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="131"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="80" t="s">
+      <c r="D10" s="120"/>
+      <c r="E10" s="121"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="146"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="81"/>
-      <c r="E11" s="82"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A12" s="131"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="83" t="s">
+      <c r="D11" s="105"/>
+      <c r="E11" s="106"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="146"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="84"/>
-      <c r="E12" s="85"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="131"/>
-      <c r="B13" s="98" t="s">
+      <c r="D12" s="108"/>
+      <c r="E12" s="109"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="146"/>
+      <c r="B13" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="100"/>
-    </row>
-    <row r="14" spans="1:5" ht="26.25" customHeight="1" thickBot="1">
+      <c r="C13" s="84"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="85"/>
+    </row>
+    <row r="14" spans="1:5" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="102"/>
-      <c r="D14" s="102"/>
-      <c r="E14" s="103"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="88"/>
     </row>
   </sheetData>
   <mergeCells count="16">
@@ -3117,112 +3766,112 @@
       <selection activeCell="B2" sqref="B2:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B2" s="59" t="s">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="128" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="61"/>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="62" t="s">
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="130"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="64"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B4" s="40" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="78"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="41"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="76"/>
       <c r="G4" s="7"/>
     </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="38" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="66"/>
-    </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B6" s="40" t="s">
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="99"/>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="41"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="67" t="s">
+      <c r="C6" s="100"/>
+      <c r="D6" s="100"/>
+      <c r="E6" s="100"/>
+      <c r="F6" s="76"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B8" s="50" t="s">
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
+      <c r="F7" s="134"/>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="52"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="53" t="s">
+      <c r="C8" s="123"/>
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="124"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="55"/>
-    </row>
-    <row r="10" spans="2:7" ht="15.75" thickBot="1">
-      <c r="B10" s="56" t="s">
+      <c r="C9" s="126"/>
+      <c r="D9" s="126"/>
+      <c r="E9" s="126"/>
+      <c r="F9" s="127"/>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="58"/>
-    </row>
-    <row r="12" spans="2:7">
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="94"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:7">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:7">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:7">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:7">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>38</v>
       </c>
@@ -3251,7 +3900,7 @@
       <selection activeCell="B2" sqref="B2:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
@@ -3260,17 +3909,17 @@
     <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B2" s="70" t="s">
+    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72"/>
-    </row>
-    <row r="3" spans="2:6">
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="64"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3287,70 +3936,70 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B4" s="76" t="s">
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="76" t="s">
+      <c r="C4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="65" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
       <c r="F5" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B6" s="121"/>
-      <c r="C6" s="121"/>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
+    <row r="6" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="66"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
       <c r="F6" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="98" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1">
-      <c r="B8" s="101" t="s">
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="85"/>
+    </row>
+    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="102"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="102"/>
-      <c r="F8" s="103"/>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="88"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" ht="27" customHeight="1"/>
+    <row r="26" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B4:B6"/>
@@ -3374,19 +4023,19 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B2" s="122" t="s">
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="137" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="123"/>
-    </row>
-    <row r="3" spans="2:3">
+      <c r="C2" s="138"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>53</v>
       </c>
@@ -3394,7 +4043,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" thickBot="1">
+    <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>54</v>
       </c>
@@ -3402,17 +4051,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15" customHeight="1">
-      <c r="B5" s="124" t="s">
+    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="139" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="125"/>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" thickBot="1">
-      <c r="B6" s="126" t="s">
+      <c r="C5" s="140"/>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="141" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="127"/>
+      <c r="C6" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3432,23 +4081,23 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="36.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:2" ht="15.75" thickBot="1">
+    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="30.75" thickBot="1">
+    <row r="4" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>58</v>
       </c>
@@ -3463,26 +4112,26 @@
   <dimension ref="B1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:2" ht="15.75" thickBot="1">
+    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="30.75" thickBot="1">
+    <row r="4" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>60</v>
       </c>
@@ -3500,22 +4149,22 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B2" s="122" t="s">
+    <row r="1" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="137" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="123"/>
-    </row>
-    <row r="3" spans="2:5" ht="45">
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="138"/>
+    </row>
+    <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>62</v>
       </c>
@@ -3529,7 +4178,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1">
+    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>63</v>
       </c>
@@ -3543,21 +4192,21 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1">
-      <c r="B5" s="124" t="s">
+    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="139" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="129"/>
-      <c r="D5" s="129"/>
-      <c r="E5" s="125"/>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B6" s="126" t="s">
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="140"/>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="141" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="130"/>
-      <c r="D6" s="130"/>
-      <c r="E6" s="127"/>
+      <c r="C6" s="145"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3577,23 +4226,23 @@
       <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:2" ht="15.75" thickBot="1">
+    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="30.75" thickBot="1">
+    <row r="4" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>70</v>
       </c>
@@ -3611,7 +4260,7 @@
       <selection activeCell="B2" sqref="B2:G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
@@ -3619,134 +4268,134 @@
     <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B2" s="112" t="s">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="114"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="72"/>
+    </row>
+    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="38" t="s">
+      <c r="E3" s="74"/>
+      <c r="F3" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="66"/>
+      <c r="G3" s="99"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="2:8" ht="27.75" thickBot="1">
+    <row r="4" spans="2:8" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="40" t="s">
+      <c r="E4" s="76"/>
+      <c r="F4" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="41"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1">
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
-    </row>
-    <row r="6" spans="2:8" ht="15" customHeight="1" thickBot="1">
-      <c r="B6" s="107" t="s">
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
+      <c r="G5" s="78"/>
+    </row>
+    <row r="6" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="44"/>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" customHeight="1">
-      <c r="B7" s="107"/>
-      <c r="C7" s="38" t="s">
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="98"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="95"/>
+      <c r="C7" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="66"/>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B8" s="107"/>
-      <c r="C8" s="40" t="s">
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="99"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="95"/>
+      <c r="C8" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="41"/>
-    </row>
-    <row r="9" spans="2:8" ht="15" customHeight="1">
-      <c r="B9" s="107"/>
-      <c r="C9" s="43" t="s">
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="76"/>
+    </row>
+    <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="95"/>
+      <c r="C9" s="97" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="44"/>
-    </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B10" s="108"/>
-      <c r="C10" s="65" t="s">
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="98"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="96"/>
+      <c r="C10" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="41"/>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="104" t="s">
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="76"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
-    </row>
-    <row r="12" spans="2:8" ht="35.25" customHeight="1" thickBot="1">
-      <c r="B12" s="56" t="s">
+      <c r="C11" s="90"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="91"/>
+    </row>
+    <row r="12" spans="2:8" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="58"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -3778,23 +4427,23 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="15.75" thickBot="1"/>
-    <row r="2" spans="2:2" ht="15.75" thickBot="1">
+    <row r="1" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="30.75" thickBot="1">
+    <row r="4" spans="2:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>51</v>
       </c>
@@ -3806,23 +4455,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f6f62870-2e10-44eb-8103-92b7757a24b0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054CC43BFDBAC2846BA8B34BC10786113" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="b57eec82f3c5f07a7c9d690ca3233865">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f6f62870-2e10-44eb-8103-92b7757a24b0" xmlns:ns4="a36d8842-b716-4d2d-94eb-9c868548fb72" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2da8a98225d4a9ceb39ead77cef7e9e4" ns3:_="" ns4:_="">
     <xsd:import namespace="f6f62870-2e10-44eb-8103-92b7757a24b0"/>
@@ -4051,32 +4683,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C538F83C-6BD1-421F-B54C-ED62748DFD95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a36d8842-b716-4d2d-94eb-9c868548fb72"/>
-    <ds:schemaRef ds:uri="f6f62870-2e10-44eb-8103-92b7757a24b0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67EF9C88-37B4-4EEF-9470-530587E01248}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f6f62870-2e10-44eb-8103-92b7757a24b0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F60F309A-64C5-4BD8-A9F1-BF8C96C0C142}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4093,4 +4717,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67EF9C88-37B4-4EEF-9470-530587E01248}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C538F83C-6BD1-421F-B54C-ED62748DFD95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a36d8842-b716-4d2d-94eb-9c868548fb72"/>
+    <ds:schemaRef ds:uri="f6f62870-2e10-44eb-8103-92b7757a24b0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>